<commit_message>
adding descriptions to acronyms
</commit_message>
<xml_diff>
--- a/Hockey Acronyms.xlsx
+++ b/Hockey Acronyms.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gonza203/Documents/Data Visualization &amp; Analytics Class Files/Final Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ravin\Downloads\Hard_Refresh\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52CB6735-F839-D443-9F67-CED8BF7B7E1A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BB11231-47B1-4393-866D-B5A751B6B0B9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="15000" xr2:uid="{BCE24C34-C86B-6D40-AC50-E5F62FB9EAEC}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{BCE24C34-C86B-6D40-AC50-E5F62FB9EAEC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="115">
   <si>
     <t>Accronym</t>
   </si>
@@ -367,13 +367,22 @@
   </si>
   <si>
     <t>Face Off Losses</t>
+  </si>
+  <si>
+    <t>Even Strength Assists</t>
+  </si>
+  <si>
+    <t>Power Play Assists</t>
+  </si>
+  <si>
+    <t>Short-Handed Assists</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -740,21 +749,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F7ADB07-F7C9-BF4A-8088-0200A331DA15}">
   <dimension ref="A1:C59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="B60" sqref="B60"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="33.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -765,7 +774,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -773,7 +782,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -781,7 +790,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -789,7 +798,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -800,7 +809,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -808,7 +817,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -816,7 +825,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -824,7 +833,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -832,7 +841,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -840,7 +849,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -851,7 +860,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -859,7 +868,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -867,7 +876,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -875,7 +884,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -883,7 +892,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -894,7 +903,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -905,7 +914,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -913,7 +922,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -921,7 +930,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>21</v>
       </c>
@@ -929,7 +938,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>22</v>
       </c>
@@ -937,7 +946,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -945,7 +954,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -956,7 +965,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>25</v>
       </c>
@@ -964,7 +973,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -972,7 +981,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>27</v>
       </c>
@@ -983,7 +992,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>28</v>
       </c>
@@ -991,7 +1000,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>29</v>
       </c>
@@ -999,7 +1008,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>30</v>
       </c>
@@ -1007,7 +1016,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>31</v>
       </c>
@@ -1015,7 +1024,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>32</v>
       </c>
@@ -1023,7 +1032,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>33</v>
       </c>
@@ -1034,7 +1043,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>34</v>
       </c>
@@ -1042,7 +1051,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>35</v>
       </c>
@@ -1053,7 +1062,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>36</v>
       </c>
@@ -1061,12 +1070,12 @@
         <v>54</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>81</v>
       </c>
@@ -1074,7 +1083,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="40" spans="1:3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>4</v>
       </c>
@@ -1082,7 +1091,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="41" spans="1:3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>5</v>
       </c>
@@ -1090,7 +1099,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="42" spans="1:3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>97</v>
       </c>
@@ -1098,7 +1107,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="43" spans="1:3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>11</v>
       </c>
@@ -1106,7 +1115,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="44" spans="1:3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" s="3" t="s">
         <v>82</v>
       </c>
@@ -1117,7 +1126,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="45" spans="1:3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>83</v>
       </c>
@@ -1125,7 +1134,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="46" spans="1:3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>84</v>
       </c>
@@ -1136,7 +1145,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="47" spans="1:3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>85</v>
       </c>
@@ -1144,7 +1153,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="48" spans="1:3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>22</v>
       </c>
@@ -1152,7 +1161,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="49" spans="1:2">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>28</v>
       </c>
@@ -1160,7 +1169,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="50" spans="1:2">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>86</v>
       </c>
@@ -1168,22 +1177,31 @@
         <v>106</v>
       </c>
     </row>
-    <row r="51" spans="1:2">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="52" spans="1:2">
+      <c r="B51" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="53" spans="1:2">
+      <c r="B52" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="54" spans="1:2">
+      <c r="B53" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>32</v>
       </c>
@@ -1191,7 +1209,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="55" spans="1:2">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>90</v>
       </c>
@@ -1199,7 +1217,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="56" spans="1:2">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>91</v>
       </c>
@@ -1207,7 +1225,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="57" spans="1:2">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>92</v>
       </c>
@@ -1215,7 +1233,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="58" spans="1:2">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>93</v>
       </c>
@@ -1223,7 +1241,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="59" spans="1:2">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>94</v>
       </c>

</xml_diff>